<commit_message>
Update upper bound of tumor size
Upper bound of size primary 1 and 2 see to 100 cm
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Incident Cases Rules/BCRPP Incident Cases Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Incident Cases Rules/BCRPP Incident Cases Warning Rules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D0E11-56FB-43A3-BC94-F949B66AEAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B1D6D-2F36-4873-9AD2-0FDE7681B1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,9 +275,6 @@
     <t>size_primary2 should be between 20 and 50 mm when sizecat_primary2 is 2</t>
   </si>
   <si>
-    <t>size_primary2 &gt;= 50 | size_primary2  == 888</t>
-  </si>
-  <si>
     <t>size_primary2 should be greater than 50 mm when sizecat_primary2 is 3</t>
   </si>
   <si>
@@ -320,7 +317,10 @@
     <t>ki67cat_primary2 does not have recognized values</t>
   </si>
   <si>
-    <t>size_primary1 &gt; 50 &amp;size_primary1 &lt;= 100 | size_primary1  == 888</t>
+    <t>size_primary1 &gt; 50 &amp; size_primary1 &lt;= 100 | size_primary1  == 888</t>
+  </si>
+  <si>
+    <t>size_primary2 &gt; 50 &amp; size_primary2 &lt;= 100 | size_primary2  == 888</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1236,7 +1236,7 @@
         <v>48</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>46</v>
@@ -1648,7 +1648,7 @@
         <v>75</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>73</v>
@@ -1668,7 +1668,7 @@
         <v>75</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
@@ -1704,12 +1704,12 @@
         <v>75</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>21</v>
@@ -1733,15 +1733,15 @@
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="T29" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="T29" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>21</v>
@@ -1765,15 +1765,15 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T30" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="T30" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>21</v>
@@ -1797,15 +1797,15 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T31" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>28</v>
@@ -1815,16 +1815,16 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1835,15 +1835,15 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>21</v>
@@ -1867,10 +1867,10 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T33" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="T33" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>